<commit_message>
Seconds displayed + updates to library
NeoMatrix + NeoPixel instances running at the same time
</commit_message>
<xml_diff>
--- a/arduino/LANGUAGE layout helper.xlsx
+++ b/arduino/LANGUAGE layout helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="3780" windowHeight="3192" activeTab="3"/>
+    <workbookView xWindow="384" yWindow="132" windowWidth="3780" windowHeight="3192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Clock_TiM" sheetId="1" r:id="rId1"/>
@@ -4068,9 +4068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J18:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4734,7 +4734,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>85</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>Row, Col, Length,   //comment</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>0</v>
       </c>
@@ -4788,15 +4788,15 @@
         <v>0, 0, 6,   //twenty</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>87</v>
@@ -4812,18 +4812,18 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" ref="J19:J57" si="0">B19&amp;C19&amp;D19&amp;E19&amp;F19&amp;G19&amp;H19</f>
-        <v>0, 8, 6,   //thirty</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+        <v>8, 0, 6,   //thirty</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>87</v>
@@ -4839,18 +4839,18 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>1, 0, 5,   //forty</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+        <v>0, 1, 5,   //forty</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>87</v>
@@ -4866,18 +4866,18 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>1, 5, 5,   //fifty</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="6">
-        <v>1</v>
+        <v>5, 1, 5,   //fifty</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D22">
-        <v>11</v>
+      <c r="D22" s="6">
+        <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>87</v>
@@ -4893,18 +4893,20 @@
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>1, 11, 3,   //ten</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="6">
-        <v>2</v>
+        <v>11, 1, 3,   //ten</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D23">
-        <v>0</v>
+      <c r="D23" s="6">
+        <v>2</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>87</v>
@@ -4920,18 +4922,20 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>2, 0, 8,   //thirteen</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="6">
-        <v>2</v>
+        <v>0, 2, 8,   //thirteen</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D24">
-        <v>8</v>
+      <c r="D24" s="6">
+        <v>2</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>87</v>
@@ -4947,18 +4951,20 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>2, 8, 3,   //one</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="6">
-        <v>2</v>
+        <v>8, 2, 3,   //one</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>11</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D25">
-        <v>11</v>
+      <c r="D25" s="6">
+        <v>2</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>87</v>
@@ -4974,18 +4980,20 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>2, 11, 3,   //two</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="6">
-        <v>3</v>
+        <v>11, 2, 3,   //two</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D26">
-        <v>0</v>
+      <c r="D26" s="6">
+        <v>3</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>87</v>
@@ -5001,18 +5009,20 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>3, 0, 4,   //four</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="6">
-        <v>3</v>
+        <v>0, 3, 4,   //four</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>0</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D27">
-        <v>0</v>
+      <c r="D27" s="6">
+        <v>3</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>87</v>
@@ -5028,18 +5038,20 @@
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>3, 0, 8,   //fourteen</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="6">
-        <v>3</v>
+        <v>0, 3, 8,   //fourteen</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>9</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D28">
-        <v>9</v>
+      <c r="D28" s="6">
+        <v>3</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>87</v>
@@ -5055,18 +5067,20 @@
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>3, 9, 4,   //five</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="6">
-        <v>4</v>
+        <v>9, 3, 4,   //five</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D29">
-        <v>0</v>
+      <c r="D29" s="6">
+        <v>4</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>87</v>
@@ -5082,18 +5096,20 @@
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>4, 0, 7,   //fifteen</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="6">
-        <v>4</v>
+        <v>0, 4, 7,   //fifteen</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>7</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D30">
-        <v>7</v>
+      <c r="D30" s="6">
+        <v>4</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>87</v>
@@ -5109,18 +5125,20 @@
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>4, 7, 3,   //six</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="6">
-        <v>4</v>
+        <v>7, 4, 3,   //six</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>7</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D31">
-        <v>7</v>
+      <c r="D31" s="6">
+        <v>4</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>87</v>
@@ -5136,18 +5154,20 @@
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>4, 7, 7,   //sixteen</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="6">
-        <v>5</v>
+        <v>7, 4, 7,   //sixteen</v>
+      </c>
+      <c r="N31" s="6"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D32">
-        <v>0</v>
+      <c r="D32" s="6">
+        <v>5</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>87</v>
@@ -5163,18 +5183,20 @@
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>5, 0, 5,   //seven</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="6">
-        <v>5</v>
+        <v>0, 5, 5,   //seven</v>
+      </c>
+      <c r="N32" s="6"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>0</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D33">
-        <v>0</v>
+      <c r="D33" s="6">
+        <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>87</v>
@@ -5190,18 +5212,20 @@
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>5, 0, 9,   //seventeen</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="6">
-        <v>5</v>
+        <v>0, 5, 9,   //seventeen</v>
+      </c>
+      <c r="N33" s="6"/>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>9</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D34">
-        <v>9</v>
+      <c r="D34" s="6">
+        <v>5</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>87</v>
@@ -5217,18 +5241,20 @@
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>5, 9, 5,   //three</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="6">
-        <v>6</v>
+        <v>9, 5, 5,   //three</v>
+      </c>
+      <c r="N34" s="6"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>0</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D35">
-        <v>0</v>
+      <c r="D35" s="6">
+        <v>6</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>87</v>
@@ -5244,18 +5270,20 @@
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>6, 0, 5,   //eight</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="6">
-        <v>6</v>
+        <v>0, 6, 5,   //eight</v>
+      </c>
+      <c r="N35" s="6"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>0</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D36">
-        <v>0</v>
+      <c r="D36" s="6">
+        <v>6</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>87</v>
@@ -5271,18 +5299,20 @@
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>6, 0, 8,   //eighteen</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="6">
-        <v>6</v>
+        <v>0, 6, 8,   //eighteen</v>
+      </c>
+      <c r="N36" s="6"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>8</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D37">
-        <v>8</v>
+      <c r="D37" s="6">
+        <v>6</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>87</v>
@@ -5298,18 +5328,20 @@
       </c>
       <c r="J37" t="str">
         <f t="shared" ref="J37:J39" si="1">B37&amp;C37&amp;D37&amp;E37&amp;F37&amp;G37&amp;H37</f>
-        <v>6, 8, 6,   //eleven</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="6">
-        <v>7</v>
+        <v>8, 6, 6,   //eleven</v>
+      </c>
+      <c r="N37" s="6"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>0</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D38">
-        <v>0</v>
+      <c r="D38" s="6">
+        <v>7</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>87</v>
@@ -5325,18 +5357,20 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="1"/>
-        <v>7, 0, 4,   //nine</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="6">
-        <v>7</v>
+        <v>0, 7, 4,   //nine</v>
+      </c>
+      <c r="N38" s="6"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>0</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D39">
-        <v>0</v>
+      <c r="D39" s="6">
+        <v>7</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>87</v>
@@ -5352,18 +5386,20 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="1"/>
-        <v>7, 0, 8,   //nineteen</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="6">
-        <v>7</v>
+        <v>0, 7, 8,   //nineteen</v>
+      </c>
+      <c r="N39" s="6"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>8</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D40">
-        <v>8</v>
+      <c r="D40" s="6">
+        <v>7</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>87</v>
@@ -5379,18 +5415,20 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>7, 8, 6,   //twelve</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="6">
-        <v>8</v>
+        <v>8, 7, 6,   //twelve</v>
+      </c>
+      <c r="N40" s="6"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D41">
-        <v>1</v>
+      <c r="D41" s="6">
+        <v>8</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>87</v>
@@ -5406,18 +5444,20 @@
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>8, 1, 6,   //minute</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="6">
-        <v>8</v>
+        <v>1, 8, 6,   //minute</v>
+      </c>
+      <c r="N41" s="6"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D42">
-        <v>1</v>
+      <c r="D42" s="6">
+        <v>8</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>87</v>
@@ -5433,18 +5473,20 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" ref="J42" si="2">B42&amp;C42&amp;D42&amp;E42&amp;F42&amp;G42&amp;H42</f>
-        <v>8, 1, 7,   //minutes</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="6">
-        <v>8</v>
+        <v>1, 8, 7,   //minutes</v>
+      </c>
+      <c r="N42" s="6"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>9</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D43">
-        <v>9</v>
+      <c r="D43" s="6">
+        <v>8</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>87</v>
@@ -5460,18 +5502,20 @@
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>8, 9, 4,   //past</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="6">
-        <v>8</v>
+        <v>9, 8, 4,   //past</v>
+      </c>
+      <c r="N43" s="6"/>
+      <c r="O43" s="4"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>12</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D44">
-        <v>12</v>
+      <c r="D44" s="6">
+        <v>8</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>87</v>
@@ -5487,18 +5531,20 @@
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>8, 12, 2,   //to</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="6">
-        <v>9</v>
+        <v>12, 8, 2,   //to</v>
+      </c>
+      <c r="N44" s="6"/>
+      <c r="O44" s="4"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>0</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D45">
-        <v>0</v>
+      <c r="D45" s="6">
+        <v>9</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>87</v>
@@ -5514,18 +5560,20 @@
       </c>
       <c r="J45" t="str">
         <f t="shared" ref="J45" si="3">B45&amp;C45&amp;D45&amp;E45&amp;F45&amp;G45&amp;H45</f>
-        <v>9, 0, 3,   //two</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="6">
-        <v>9</v>
+        <v>0, 9, 3,   //two</v>
+      </c>
+      <c r="N45" s="6"/>
+      <c r="O45" s="4"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>2</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D46">
-        <v>2</v>
+      <c r="D46" s="6">
+        <v>9</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>87</v>
@@ -5541,18 +5589,20 @@
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>9, 2, 3,   //one</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="6">
-        <v>9</v>
+        <v>2, 9, 3,   //one</v>
+      </c>
+      <c r="N46" s="6"/>
+      <c r="O46" s="4"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>4</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D47">
-        <v>4</v>
+      <c r="D47" s="6">
+        <v>9</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>87</v>
@@ -5568,18 +5618,20 @@
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>9, 4, 3,   //eight</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="6">
-        <v>9</v>
+        <v>4, 9, 3,   //eight</v>
+      </c>
+      <c r="N47" s="6"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>8</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D48">
-        <v>8</v>
+      <c r="D48" s="6">
+        <v>9</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>87</v>
@@ -5595,18 +5647,20 @@
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>9, 8, 3,   //ten</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="6">
-        <v>9</v>
+        <v>8, 9, 3,   //ten</v>
+      </c>
+      <c r="N48" s="6"/>
+      <c r="O48" s="4"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>11</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D49">
-        <v>11</v>
+      <c r="D49" s="6">
+        <v>9</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>87</v>
@@ -5622,18 +5676,20 @@
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>9, 11, 5,   //six</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="6">
-        <v>10</v>
+        <v>11, 9, 5,   //six</v>
+      </c>
+      <c r="N49" s="6"/>
+      <c r="O49" s="4"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>0</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D50">
-        <v>0</v>
+      <c r="D50" s="6">
+        <v>10</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>87</v>
@@ -5649,18 +5705,20 @@
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>10, 0, 5,   //three</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="6">
-        <v>10</v>
+        <v>0, 10, 5,   //three</v>
+      </c>
+      <c r="N50" s="6"/>
+      <c r="O50" s="4"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>5</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D51">
-        <v>5</v>
+      <c r="D51" s="6">
+        <v>10</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>87</v>
@@ -5676,18 +5734,20 @@
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>10, 5, 4,   //nine</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="6">
-        <v>10</v>
+        <v>5, 10, 4,   //nine</v>
+      </c>
+      <c r="N51" s="6"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>8</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D52">
-        <v>8</v>
+      <c r="D52" s="6">
+        <v>10</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>87</v>
@@ -5703,18 +5763,20 @@
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>10, 8, 6,   //eleven</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="6">
-        <v>11</v>
+        <v>8, 10, 6,   //eleven</v>
+      </c>
+      <c r="N52" s="6"/>
+      <c r="O52" s="4"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>0</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D53">
-        <v>0</v>
+      <c r="D53" s="6">
+        <v>11</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>87</v>
@@ -5730,18 +5792,20 @@
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>11, 0, 4,   //four</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="6">
-        <v>11</v>
+        <v>0, 11, 4,   //four</v>
+      </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="4"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>4</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D54">
-        <v>4</v>
+      <c r="D54" s="6">
+        <v>11</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>87</v>
@@ -5757,18 +5821,20 @@
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>11, 4, 4,   //five</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="6">
-        <v>11</v>
+        <v>4, 11, 4,   //five</v>
+      </c>
+      <c r="N54" s="6"/>
+      <c r="O54" s="4"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>8</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D55">
-        <v>8</v>
+      <c r="D55" s="6">
+        <v>11</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>87</v>
@@ -5784,18 +5850,20 @@
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>11, 8, 6,   //twelve</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="6">
-        <v>12</v>
+        <v>8, 11, 6,   //twelve</v>
+      </c>
+      <c r="N55" s="6"/>
+      <c r="O55" s="4"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>0</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D56">
-        <v>0</v>
+      <c r="D56" s="6">
+        <v>12</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>87</v>
@@ -5811,18 +5879,20 @@
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
-        <v>12, 0, 5,   //seven</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="6">
-        <v>12</v>
+        <v>0, 12, 5,   //seven</v>
+      </c>
+      <c r="N56" s="6"/>
+      <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>8</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D57">
-        <v>8</v>
+      <c r="D57" s="6">
+        <v>12</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>87</v>
@@ -5838,8 +5908,10 @@
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>12, 8, 6,   //oclock</v>
-      </c>
+        <v>8, 12, 6,   //oclock</v>
+      </c>
+      <c r="N57" s="6"/>
+      <c r="O57" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7572,7 +7644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>